<commit_message>
Commit 12 - Fixed Error on saving all records for each subcategory on the category csv file / Fixed Category XLS listing first records as header
</commit_message>
<xml_diff>
--- a/INI/Jumbo_SubCategoriesPerSection.xlsx
+++ b/INI/Jumbo_SubCategoriesPerSection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pol\OneDrive\MASTER_FILES\My Documents\2022_P0\G_MED_SUPERMARKET\INI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ottel\OneDrive\MASTER_FILES\My Documents\2022_P0\G_MED_SUPERMARKET\INI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D58FD5C-2EEC-4827-B5BB-2AA2AA883390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1FCBC5-4B56-429D-94AD-B2B06537E3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="2805" windowWidth="15375" windowHeight="7875" xr2:uid="{EAC1FFFA-8500-4B28-A076-13F02CDBD5FE}"/>
+    <workbookView xWindow="4110" yWindow="3975" windowWidth="21600" windowHeight="11325" xr2:uid="{C8C3DE41-D5E5-4E59-BFB4-D3A6D674A251}"/>
   </bookViews>
   <sheets>
     <sheet name="limpieza-de-cocina" sheetId="17" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="367">
   <si>
     <t>Pollos</t>
   </si>
@@ -197,6 +197,15 @@
     <t>pescado-fresco</t>
   </si>
   <si>
+    <t>Sushi</t>
+  </si>
+  <si>
+    <t>https://www.tiendasjumbo.co/supermercado/pescados-y-mariscos/sushi?initialMap=c,c&amp;initialQuery=supermercado/pescados-y-mariscos&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
+  </si>
+  <si>
+    <t>sushi</t>
+  </si>
+  <si>
     <t>Elaborados</t>
   </si>
   <si>
@@ -206,15 +215,6 @@
     <t>elaborados</t>
   </si>
   <si>
-    <t>Sushi</t>
-  </si>
-  <si>
-    <t>https://www.tiendasjumbo.co/supermercado/pescados-y-mariscos/sushi?initialMap=c,c&amp;initialQuery=supermercado/pescados-y-mariscos&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
-  </si>
-  <si>
-    <t>sushi</t>
-  </si>
-  <si>
     <t>Mariscos</t>
   </si>
   <si>
@@ -695,6 +695,15 @@
     <t>comida-rapida</t>
   </si>
   <si>
+    <t>Apanados</t>
+  </si>
+  <si>
+    <t>https://www.tiendasjumbo.co/supermercado/platos-preparados/apanados?initialMap=c,c&amp;initialQuery=supermercado/platos-preparados&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
+  </si>
+  <si>
+    <t>apanados</t>
+  </si>
+  <si>
     <t>Verduras Congeladas</t>
   </si>
   <si>
@@ -704,15 +713,6 @@
     <t>verduras-congeladas</t>
   </si>
   <si>
-    <t>Apanados</t>
-  </si>
-  <si>
-    <t>https://www.tiendasjumbo.co/supermercado/platos-preparados/apanados?initialMap=c,c&amp;initialQuery=supermercado/platos-preparados&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
-  </si>
-  <si>
-    <t>apanados</t>
-  </si>
-  <si>
     <t>Detergentes</t>
   </si>
   <si>
@@ -920,6 +920,15 @@
     <t>afeitado</t>
   </si>
   <si>
+    <t>Cuidado De Pies</t>
+  </si>
+  <si>
+    <t>https://www.tiendasjumbo.co/supermercado/cuidado-personal/cuidado-de-pies?initialMap=c,c&amp;initialQuery=supermercado/cuidado-personal&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
+  </si>
+  <si>
+    <t>cuidado-de-pies</t>
+  </si>
+  <si>
     <t>Papel Higiénico</t>
   </si>
   <si>
@@ -929,15 +938,6 @@
     <t>papel-higienico</t>
   </si>
   <si>
-    <t>Cuidado De Pies</t>
-  </si>
-  <si>
-    <t>https://www.tiendasjumbo.co/supermercado/cuidado-personal/cuidado-de-pies?initialMap=c,c&amp;initialQuery=supermercado/cuidado-personal&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
-  </si>
-  <si>
-    <t>cuidado-de-pies</t>
-  </si>
-  <si>
     <t>Gel Y Fijadores</t>
   </si>
   <si>
@@ -1143,6 +1143,15 @@
   </si>
   <si>
     <t>guantes</t>
+  </si>
+  <si>
+    <t>Toallas y Paños De Cocina</t>
+  </si>
+  <si>
+    <t>https://www.tiendasjumbo.co/supermercado/limpieza-de-cocina/toallas-y-panos-de-cocina?initialMap=c,c&amp;initialQuery=supermercado/limpieza-de-cocina&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
+  </si>
+  <si>
+    <t>toallas-y-panos-de-cocina</t>
   </si>
 </sst>
 </file>
@@ -1493,8 +1502,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB26A2C-0C26-4B3B-9CE9-9E69C1397B4B}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3118CBA7-7198-48EF-9831-1F7E1F2245E7}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1584,13 +1593,27 @@
         <v>363</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B7" t="s">
+        <v>365</v>
+      </c>
+      <c r="C7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D7" t="s">
+        <v>366</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124FBA64-0B16-4C64-AE96-2B188A582B60}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94379450-7CB0-4390-942E-2081A76FA041}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1659,7 +1682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B336995-6C52-478C-8540-7336668C2A0C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BBD1F9-70BF-4429-AAD8-A8B590FC37F6}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1812,7 +1835,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B2671D-9CD3-4186-AC5A-C34F8AA11C9E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE0A3F4-ED33-4DAF-88DA-B36E77F1607D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1881,7 +1904,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C3E690-B8F9-4B28-AF27-85FA5DCE417C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AEF7C24-A7DA-4CD4-ADB3-679AB2F17E4F}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2034,7 +2057,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBBE3FB4-7E8A-4596-B07E-122A2921311E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56B6110-EFAB-4D44-AFFA-EE40BB0EA7B0}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2117,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07B024F-CEA6-46E0-9D4B-8C0211F0E940}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB1F7E2B-5607-4F9C-9A40-58C445F3BAAD}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2200,7 +2223,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F27763-EADD-4D4F-8BC9-F984EFB1A32F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1BAA3D-A33F-4834-BAFE-BF7539258BC7}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2325,7 +2348,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBA52B2-8894-49C9-B9DA-C424F72CC679}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD815C4-D0A4-4FC8-BDDA-4FBC5D566F0E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2337,7 +2360,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69E2433-D7F1-47D8-AA35-A26292ACF6B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4528BB9E-0324-4733-B66F-18D48FAED796}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2476,7 +2499,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D3A854-080E-4DC4-9294-01BA740E0AA9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8239BC93-2B00-4885-83E1-60CE0E7C3E0F}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2573,7 +2596,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB7FF3F-FD60-4668-8C19-9B23221158CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38F40C5-F77C-49D9-BA91-DC9DAF107C5C}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2726,7 +2749,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603BF835-1270-4A62-BD7A-1E4FA7C9ECD8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9DE24BE-FC07-4CEE-8EF1-83880BE139E1}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2865,7 +2888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB39BCC-044D-4B66-B748-8665E4432027}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62949FDE-951B-4A71-A20C-1754F821C839}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2962,7 +2985,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2D2DC5-D4FA-4A60-BDA6-288130E247E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01F4482-250A-436D-939F-D0349C0B336C}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3115,7 +3138,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDE9294-8021-441D-8ACC-1891552AB87D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC29EE7F-6610-4BA8-B550-92B6B264FF97}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3226,7 +3249,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6CC479-F34B-4C1A-8118-87C3A84EEDC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4F454E-07EB-41FC-9B48-C205D8BDF192}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Commit 14 - Test Run Completed. New feature to select section/category to run. Long run working as expected.
</commit_message>
<xml_diff>
--- a/INI/Jumbo_SubCategoriesPerSection.xlsx
+++ b/INI/Jumbo_SubCategoriesPerSection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ottel\OneDrive\MASTER_FILES\My Documents\2022_P0\G_MED_SUPERMARKET\INI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f8c66d4695cab21/MASTER_FILES/My Documents/2022_P0/G_MED_SUPERMARKET/INI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1FCBC5-4B56-429D-94AD-B2B06537E3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0D58FD5C-2EEC-4827-B5BB-2AA2AA883390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF0776BE-6046-4A09-B373-E641D41FA4D4}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="3975" windowWidth="21600" windowHeight="11325" xr2:uid="{C8C3DE41-D5E5-4E59-BFB4-D3A6D674A251}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15540" xr2:uid="{EAC1FFFA-8500-4B28-A076-13F02CDBD5FE}"/>
   </bookViews>
   <sheets>
     <sheet name="limpieza-de-cocina" sheetId="17" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="364">
   <si>
     <t>Pollos</t>
   </si>
@@ -197,6 +197,15 @@
     <t>pescado-fresco</t>
   </si>
   <si>
+    <t>Elaborados</t>
+  </si>
+  <si>
+    <t>https://www.tiendasjumbo.co/supermercado/pescados-y-mariscos/elaborados?initialMap=c,c&amp;initialQuery=supermercado/pescados-y-mariscos&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
+  </si>
+  <si>
+    <t>elaborados</t>
+  </si>
+  <si>
     <t>Sushi</t>
   </si>
   <si>
@@ -206,15 +215,6 @@
     <t>sushi</t>
   </si>
   <si>
-    <t>Elaborados</t>
-  </si>
-  <si>
-    <t>https://www.tiendasjumbo.co/supermercado/pescados-y-mariscos/elaborados?initialMap=c,c&amp;initialQuery=supermercado/pescados-y-mariscos&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
-  </si>
-  <si>
-    <t>elaborados</t>
-  </si>
-  <si>
     <t>Mariscos</t>
   </si>
   <si>
@@ -695,6 +695,15 @@
     <t>comida-rapida</t>
   </si>
   <si>
+    <t>Verduras Congeladas</t>
+  </si>
+  <si>
+    <t>https://www.tiendasjumbo.co/supermercado/platos-preparados/verduras-congeladas?initialMap=c,c&amp;initialQuery=supermercado/platos-preparados&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
+  </si>
+  <si>
+    <t>verduras-congeladas</t>
+  </si>
+  <si>
     <t>Apanados</t>
   </si>
   <si>
@@ -704,15 +713,6 @@
     <t>apanados</t>
   </si>
   <si>
-    <t>Verduras Congeladas</t>
-  </si>
-  <si>
-    <t>https://www.tiendasjumbo.co/supermercado/platos-preparados/verduras-congeladas?initialMap=c,c&amp;initialQuery=supermercado/platos-preparados&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
-  </si>
-  <si>
-    <t>verduras-congeladas</t>
-  </si>
-  <si>
     <t>Detergentes</t>
   </si>
   <si>
@@ -920,6 +920,15 @@
     <t>afeitado</t>
   </si>
   <si>
+    <t>Papel Higiénico</t>
+  </si>
+  <si>
+    <t>https://www.tiendasjumbo.co/supermercado/cuidado-personal/papel-higienico?initialMap=c,c&amp;initialQuery=supermercado/cuidado-personal&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
+  </si>
+  <si>
+    <t>papel-higienico</t>
+  </si>
+  <si>
     <t>Cuidado De Pies</t>
   </si>
   <si>
@@ -929,15 +938,6 @@
     <t>cuidado-de-pies</t>
   </si>
   <si>
-    <t>Papel Higiénico</t>
-  </si>
-  <si>
-    <t>https://www.tiendasjumbo.co/supermercado/cuidado-personal/papel-higienico?initialMap=c,c&amp;initialQuery=supermercado/cuidado-personal&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
-  </si>
-  <si>
-    <t>papel-higienico</t>
-  </si>
-  <si>
     <t>Gel Y Fijadores</t>
   </si>
   <si>
@@ -1143,15 +1143,6 @@
   </si>
   <si>
     <t>guantes</t>
-  </si>
-  <si>
-    <t>Toallas y Paños De Cocina</t>
-  </si>
-  <si>
-    <t>https://www.tiendasjumbo.co/supermercado/limpieza-de-cocina/toallas-y-panos-de-cocina?initialMap=c,c&amp;initialQuery=supermercado/limpieza-de-cocina&amp;map=category-1,category-2,category-3&amp;order=OrderByNameASC</t>
-  </si>
-  <si>
-    <t>toallas-y-panos-de-cocina</t>
   </si>
 </sst>
 </file>
@@ -1502,12 +1493,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3118CBA7-7198-48EF-9831-1F7E1F2245E7}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB26A2C-0C26-4B3B-9CE9-9E69C1397B4B}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1591,20 +1587,6 @@
       </c>
       <c r="D6" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>364</v>
-      </c>
-      <c r="B7" t="s">
-        <v>365</v>
-      </c>
-      <c r="C7" t="s">
-        <v>347</v>
-      </c>
-      <c r="D7" t="s">
-        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -1613,7 +1595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94379450-7CB0-4390-942E-2081A76FA041}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124FBA64-0B16-4C64-AE96-2B188A582B60}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1682,7 +1664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BBD1F9-70BF-4429-AAD8-A8B590FC37F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B336995-6C52-478C-8540-7336668C2A0C}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1835,7 +1817,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE0A3F4-ED33-4DAF-88DA-B36E77F1607D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B2671D-9CD3-4186-AC5A-C34F8AA11C9E}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1904,7 +1886,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AEF7C24-A7DA-4CD4-ADB3-679AB2F17E4F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C3E690-B8F9-4B28-AF27-85FA5DCE417C}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2057,7 +2039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56B6110-EFAB-4D44-AFFA-EE40BB0EA7B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBBE3FB4-7E8A-4596-B07E-122A2921311E}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2140,7 +2122,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB1F7E2B-5607-4F9C-9A40-58C445F3BAAD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07B024F-CEA6-46E0-9D4B-8C0211F0E940}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2223,12 +2205,17 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1BAA3D-A33F-4834-BAFE-BF7539258BC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F27763-EADD-4D4F-8BC9-F984EFB1A32F}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="193.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2348,7 +2335,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD815C4-D0A4-4FC8-BDDA-4FBC5D566F0E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBA52B2-8894-49C9-B9DA-C424F72CC679}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2360,7 +2347,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4528BB9E-0324-4733-B66F-18D48FAED796}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69E2433-D7F1-47D8-AA35-A26292ACF6B6}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2499,7 +2486,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8239BC93-2B00-4885-83E1-60CE0E7C3E0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D3A854-080E-4DC4-9294-01BA740E0AA9}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2596,7 +2583,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38F40C5-F77C-49D9-BA91-DC9DAF107C5C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB7FF3F-FD60-4668-8C19-9B23221158CA}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2749,7 +2736,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9DE24BE-FC07-4CEE-8EF1-83880BE139E1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603BF835-1270-4A62-BD7A-1E4FA7C9ECD8}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2888,7 +2875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62949FDE-951B-4A71-A20C-1754F821C839}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB39BCC-044D-4B66-B748-8665E4432027}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2985,7 +2972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01F4482-250A-436D-939F-D0349C0B336C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2D2DC5-D4FA-4A60-BDA6-288130E247E2}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3138,7 +3125,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC29EE7F-6610-4BA8-B550-92B6B264FF97}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDE9294-8021-441D-8ACC-1891552AB87D}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3249,7 +3236,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4F454E-07EB-41FC-9B48-C205D8BDF192}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6CC479-F34B-4C1A-8118-87C3A84EEDC6}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>